<commit_message>
Outlet pdfoutput / mechanism query + pdf FrontView filename change
</commit_message>
<xml_diff>
--- a/excel/excelOrder65.xlsx
+++ b/excel/excelOrder65.xlsx
@@ -16,12 +16,108 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="2">
-  <si>
-    <t>OVER</t>
-  </si>
-  <si>
-    <t>!</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="34">
+  <si>
+    <t>Contact</t>
+  </si>
+  <si>
+    <t>Test User User</t>
+  </si>
+  <si>
+    <t>Data of Estimate:</t>
+  </si>
+  <si>
+    <t>Sales Rep:</t>
+  </si>
+  <si>
+    <t>Firm:</t>
+  </si>
+  <si>
+    <t>Project Number:</t>
+  </si>
+  <si>
+    <t>Region:</t>
+  </si>
+  <si>
+    <t>Address:</t>
+  </si>
+  <si>
+    <t>Project Name:</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>user@user.com</t>
+  </si>
+  <si>
+    <t>Project Address:</t>
+  </si>
+  <si>
+    <t>Lead Time:</t>
+  </si>
+  <si>
+    <t>8-10 WEEKS UPON ORDER APPROVAL AND RECEIPT OF DEPOSIT</t>
+  </si>
+  <si>
+    <t>Phone Number</t>
+  </si>
+  <si>
+    <t>ROOM</t>
+  </si>
+  <si>
+    <t>REF #</t>
+  </si>
+  <si>
+    <t>QTY</t>
+  </si>
+  <si>
+    <t>FINISH</t>
+  </si>
+  <si>
+    <t>SIZE</t>
+  </si>
+  <si>
+    <t>PLATE COST</t>
+  </si>
+  <si>
+    <t>MECHANISM TYPE/QTY</t>
+  </si>
+  <si>
+    <t>MECHANISM PROVIDED BY</t>
+  </si>
+  <si>
+    <t>V&amp;VERSER COST</t>
+  </si>
+  <si>
+    <t>TOTAL # ENGRAVING</t>
+  </si>
+  <si>
+    <t>ENGRAVING COST</t>
+  </si>
+  <si>
+    <t>BACK BOX</t>
+  </si>
+  <si>
+    <t>MELKIT</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>EDGES: STRAIGHT / BEVELED</t>
+  </si>
+  <si>
+    <t>FC3008A-A1100141FA</t>
+  </si>
+  <si>
+    <t>$</t>
+  </si>
+  <si>
+    <t>MELJAC</t>
+  </si>
+  <si>
+    <t>TBD</t>
   </si>
 </sst>
 </file>
@@ -29,9 +125,18 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="1"/>
       <i val="0"/>
       <strike val="0"/>
       <u val="none"/>
@@ -57,8 +162,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
   </cellXfs>
@@ -360,42 +468,162 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
+    <row r="2" spans="1:15">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I2"/>
+      <c r="L2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="M2"/>
     </row>
-    <row r="2" spans="1:1">
-      <c r="A2">
+    <row r="3" spans="1:15">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3"/>
+      <c r="G3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3"/>
+      <c r="L3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M3"/>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4"/>
+      <c r="G4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I4"/>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5"/>
+      <c r="L5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M5" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="3" spans="1:1">
-      <c r="A3">
+    <row r="6" spans="1:15">
+      <c r="A6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6"/>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="A8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="A9"/>
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9"/>
+      <c r="E9"/>
+      <c r="F9" t="s">
+        <v>31</v>
+      </c>
+      <c r="G9"/>
+      <c r="H9" t="s">
+        <v>32</v>
+      </c>
+      <c r="I9" t="s">
+        <v>31</v>
+      </c>
+      <c r="J9">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:1">
-      <c r="A4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1">
-      <c r="A5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1">
-      <c r="A6" t="s">
-        <v>1</v>
+      <c r="K9" t="s">
+        <v>31</v>
+      </c>
+      <c r="L9" t="s">
+        <v>31</v>
+      </c>
+      <c r="M9" t="s">
+        <v>31</v>
+      </c>
+      <c r="N9" t="s">
+        <v>31</v>
+      </c>
+      <c r="O9" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>